<commit_message>
Add a version number to the templates
Allows for evolution of the template format
</commit_message>
<xml_diff>
--- a/import_specifications/templates/import_specifications.xlsx
+++ b/import_specifications/templates/import_specifications.xlsx
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t xml:space="preserve">Data type:</t>
   </si>
   <si>
     <t xml:space="preserve">assembly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version:</t>
   </si>
   <si>
     <t xml:space="preserve">staging_file_subdir_path</t>
@@ -301,7 +304,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,33 +320,39 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -365,7 +374,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -379,53 +388,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -447,7 +462,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -461,59 +476,65 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -535,7 +556,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,71 +570,77 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -635,7 +662,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -649,53 +676,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +750,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -731,53 +764,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update import spec templates
* Updated header line 1 to new format
* Regenerated the genbank uploader for new spec
</commit_message>
<xml_diff>
--- a/import_specifications/templates/import_specifications.xlsx
+++ b/import_specifications/templates/import_specifications.xlsx
@@ -25,15 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
-  <si>
-    <t xml:space="preserve">Data type:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assembly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+  <si>
+    <t xml:space="preserve">Data type: assembly; Columns: 4; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">staging_file_subdir_path</t>
@@ -60,7 +54,7 @@
     <t xml:space="preserve">Minimum contig length</t>
   </si>
   <si>
-    <t xml:space="preserve">fastq_reads_interleaved</t>
+    <t xml:space="preserve">Data type: fastq_reads_interleaved; Columns: 7; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">fastq_fwd_staging_file_name</t>
@@ -105,7 +99,7 @@
     <t xml:space="preserve">Mean Insert Size</t>
   </si>
   <si>
-    <t xml:space="preserve">fastq_reads_noninterleaved</t>
+    <t xml:space="preserve">Data type: fastq_reads_noninterleaved; Columns: 8; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">fastq_rev_staging_file_name</t>
@@ -114,15 +108,72 @@
     <t xml:space="preserve">Reverse/Right FASTQ File Path</t>
   </si>
   <si>
-    <t xml:space="preserve">genbank_genome</t>
+    <t xml:space="preserve">Data type: genbank_genome; Columns: 9; Version: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> genome_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> genome_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> source</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> scientific_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> release</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> genetic_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> generate_ids_if_needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> generate_missing_genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GenBank File Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Genome Object Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Genome Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Source of the GenBank File</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Scientific Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Release or Version of the Source Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Genetic Code for the Organism</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Generate Feature IDs if Needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spoof Genes for parentless CDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data type: gff_metagenome; Columns: 7; Version: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fasta_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gff_file</t>
   </si>
   <si>
     <t xml:space="preserve">genome_name</t>
   </si>
   <si>
-    <t xml:space="preserve">genome_type</t>
-  </si>
-  <si>
     <t xml:space="preserve">source</t>
   </si>
   <si>
@@ -132,73 +183,31 @@
     <t xml:space="preserve">genetic_code</t>
   </si>
   <si>
-    <t xml:space="preserve">scientific_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taxon_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generate_ids_if_needed</t>
-  </si>
-  <si>
     <t xml:space="preserve">generate_missing_genes</t>
   </si>
   <si>
-    <t xml:space="preserve">GenBank File Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genome Object Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genome Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source of the GenBank File</t>
+    <t xml:space="preserve">FASTA File Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GFF3 File Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metagenome Object Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source of metagenome</t>
   </si>
   <si>
     <t xml:space="preserve">Release or Version of the Source Data</t>
   </si>
   <si>
-    <t xml:space="preserve">Genetic Code for the Organism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scientific Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxonomy ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generate Feature IDs if Needed</t>
+    <t xml:space="preserve">Genetic Code for protein translation</t>
   </si>
   <si>
     <t xml:space="preserve">Spoof Genes for parentless CDS</t>
   </si>
   <si>
-    <t xml:space="preserve">gff_metagenome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fasta_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gff_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FASTA File Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GFF3 File Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metagenome Object Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source of metagenome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genetic Code for protein translation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sra_reads</t>
+    <t xml:space="preserve">Data type: sra_reads; Columns: 7; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">sra_staging_file_name</t>
@@ -317,42 +326,33 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -385,62 +385,53 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -473,68 +464,59 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -553,7 +535,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -567,80 +549,65 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -673,62 +640,53 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="G2" s="0" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -761,62 +719,53 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>